<commit_message>
compute the fraction BB:BP
</commit_message>
<xml_diff>
--- a/Data/Meta.xlsx
+++ b/Data/Meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhachaichi\Documents\Virtual_Water_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28946353-3E2A-48B9-A562-C5C7E5DDDC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82EB11F-9761-48F2-BE40-7D599C68BF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Eora_classification</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Wholesale Trade</t>
-  </si>
-  <si>
-    <t>Business</t>
   </si>
   <si>
     <t>Retail Trade</t>
@@ -468,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F95F9A-872A-4A62-938B-EF17B44FD883}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -627,7 +624,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -660,7 +657,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -668,10 +665,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -679,7 +676,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -701,7 +698,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -712,7 +709,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -723,7 +720,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -734,7 +731,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -756,10 +753,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>21</v>
@@ -767,7 +764,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>

</xml_diff>